<commit_message>
preprocesado producción memoria, ann pruebas
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB53A6FF-8794-4815-8A87-6EABB596BD52}"/>
   <bookViews>
-    <workbookView xWindow="14085" yWindow="4920" windowWidth="23460" windowHeight="10950"/>
+    <workbookView xWindow="5340" yWindow="5040" windowWidth="23460" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -75,12 +75,18 @@
   </si>
   <si>
     <t>0.9820</t>
+  </si>
+  <si>
+    <t>Best Accuracy: 98.20 % Best Parameters: {'activation': 'tanh', 'hidden_layer_sizes': (7, 7, 1), 'learning_rate': 'constant', 'solver': 'adam'}</t>
+  </si>
+  <si>
+    <t>APLICACIÓN DE GRID SEARCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,10 +151,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,9 +165,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,40 +491,46 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="L6" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -537,27 +550,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>50</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>8</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>30948</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>191</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -565,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -581,7 +594,7 @@
       <c r="E14">
         <v>260</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
svm y ann done
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EBD82B7-4FD1-49A9-80DA-F2FC86918720}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168AA01B-4DD5-4D0E-8765-10951BB99AB4}"/>
   <bookViews>
-    <workbookView xWindow="14670" yWindow="1935" windowWidth="23460" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2610" yWindow="570" windowWidth="17655" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>0.0695</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>0.9780</t>
   </si>
 </sst>
 </file>
@@ -211,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,7 +235,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L30"/>
+  <dimension ref="A2:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,10 +839,10 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26">
         <v>376378</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26">
         <v>1606</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -885,11 +890,57 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
+    <row r="36" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>377074</v>
+      </c>
+      <c r="E38">
+        <v>639</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="H7:K7"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="H37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fin graficas cap 3
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6134A0D1-DBF9-4070-B788-85ECE8E383DD}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5C6E31-A177-4A47-A48C-D5876AC315A2}"/>
   <bookViews>
     <workbookView xWindow="10590" yWindow="1335" windowWidth="17655" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>0.01</t>
+  </si>
+  <si>
+    <t>0.9778</t>
   </si>
 </sst>
 </file>
@@ -268,16 +271,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,29 +613,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -936,14 +939,14 @@
       <c r="G30" s="2"/>
     </row>
     <row r="36" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
@@ -967,10 +970,10 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="7" t="s">
+      <c r="L37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M37" s="7"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D38">
@@ -984,6 +987,12 @@
       </c>
       <c r="H38" t="s">
         <v>33</v>
+      </c>
+      <c r="L38" t="s">
+        <v>44</v>
+      </c>
+      <c r="M38" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1017,14 +1026,14 @@
       <c r="L41" s="4"/>
     </row>
     <row r="48" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -1048,10 +1057,10 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-      <c r="L49" s="7" t="s">
+      <c r="L49" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M49" s="7"/>
+      <c r="M49" s="8"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D50">
@@ -1095,15 +1104,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="H37:K37"/>
     <mergeCell ref="A48:F48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
random forest fin pruebas, trees dot
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5C6E31-A177-4A47-A48C-D5876AC315A2}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CFB65E7-A16A-4F82-908B-DA5C28A856AA}"/>
   <bookViews>
-    <workbookView xWindow="10590" yWindow="1335" windowWidth="17655" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1650" yWindow="1020" windowWidth="17655" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -140,12 +140,6 @@
     <t>SIN PCA</t>
   </si>
   <si>
-    <t>CON PCA</t>
-  </si>
-  <si>
-    <t>FALTA HACER GRID SEARCH Y KFOLD</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -171,6 +165,67 @@
   </si>
   <si>
     <t>0.9778</t>
+  </si>
+  <si>
+    <t>n_estimators = 10, criterion = 'entropy'</t>
+  </si>
+  <si>
+    <t>parameters = {#'n_estimators': [1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15], 
+    'criterion': ['entropy', 'gini']    }</t>
+  </si>
+  <si>
+    <t>Se utiliza el de 10, no es necesario aumentar la complejidad para mejorar la precisión</t>
+  </si>
+  <si>
+    <t>GRID SEARCH -&gt; Best Accuracy: 99.23 %,  Best Parameters: {'criterion': 'entropy', 'n_estimators': 50} (83 min)</t>
+  </si>
+  <si>
+    <t>GRID SEARCH -&gt; Best Accuracy: 99.18 %, Best Parameters: {'criterion': 'gini', 'n_estimators': 15} (mas de 83 min)</t>
+  </si>
+  <si>
+    <t>0.9779</t>
+  </si>
+  <si>
+    <t>CON PCA (2)</t>
+  </si>
+  <si>
+    <t>CON PCA (3)</t>
+  </si>
+  <si>
+    <t>0.9764</t>
+  </si>
+  <si>
+    <t>% (cm)</t>
+  </si>
+  <si>
+    <t>SIN PCA Y FS</t>
+  </si>
+  <si>
+    <t>CON FS (5)</t>
+  </si>
+  <si>
+    <t>CON FS (8)</t>
+  </si>
+  <si>
+    <t>['cap', 'dist', 'origen_id', 'dest_id', 'len_origen_tag', 'len_dest_tag,  'total_balance', 'abs_flux']</t>
+  </si>
+  <si>
+    <t>['cap', 'len_origen_tag', 'len_dest_tag', 'Beam Irradiance (W/m2)', 'Plane of Array Irradiance (W/m2)']</t>
+  </si>
+  <si>
+    <t>0.9763</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0.9773</t>
+  </si>
+  <si>
+    <t>0.9769</t>
+  </si>
+  <si>
+    <t>0.9765</t>
   </si>
 </sst>
 </file>
@@ -261,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,8 +335,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M51"/>
+  <dimension ref="A2:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
@@ -970,10 +1032,10 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="M37" s="8"/>
+      <c r="L37" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D38">
@@ -989,10 +1051,10 @@
         <v>33</v>
       </c>
       <c r="L38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1002,13 +1064,16 @@
       <c r="E39">
         <v>0</v>
       </c>
+      <c r="F39" t="s">
+        <v>62</v>
+      </c>
       <c r="H39" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1027,7 +1092,7 @@
     </row>
     <row r="48" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1035,79 +1100,230 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1" t="s">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="F53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="H53" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="8" t="s">
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M53" s="9"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>376752</v>
+      </c>
+      <c r="E54">
+        <v>6092</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L54" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54" t="s">
         <v>38</v>
       </c>
-      <c r="M49" s="8"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D50">
-        <v>376752</v>
-      </c>
-      <c r="E50">
-        <v>6092</v>
-      </c>
-      <c r="F50" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" t="s">
-        <v>33</v>
-      </c>
-      <c r="L50" t="s">
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>376593</v>
+      </c>
+      <c r="E55">
+        <v>50</v>
+      </c>
+      <c r="F55" t="s">
         <v>39</v>
       </c>
-      <c r="M50" t="s">
+      <c r="H55" t="s">
+        <v>49</v>
+      </c>
+      <c r="L55" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D51">
-        <v>376593</v>
-      </c>
-      <c r="E51">
+      <c r="M55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>376965</v>
+      </c>
+      <c r="E56">
+        <v>136</v>
+      </c>
+      <c r="F56" t="s">
+        <v>51</v>
+      </c>
+      <c r="H56" t="s">
         <v>50</v>
       </c>
-      <c r="F51" t="s">
+      <c r="L56" t="s">
+        <v>58</v>
+      </c>
+      <c r="M56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>376555</v>
+      </c>
+      <c r="E57">
+        <v>1137</v>
+      </c>
+      <c r="F57" t="s">
+        <v>48</v>
+      </c>
+      <c r="H57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" t="s">
+        <v>48</v>
+      </c>
+      <c r="M57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>374986</v>
+      </c>
+      <c r="E58">
+        <v>2461</v>
+      </c>
+      <c r="F58" t="s">
+        <v>60</v>
+      </c>
+      <c r="H58" t="s">
+        <v>55</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M58" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H51" t="s">
-        <v>34</v>
-      </c>
-      <c r="L51" t="s">
-        <v>42</v>
-      </c>
-      <c r="M51" t="s">
-        <v>43</v>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="N64" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+      <c r="R65" s="8"/>
+      <c r="S65" s="8"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="L49:M49"/>
+  <mergeCells count="12">
+    <mergeCell ref="N64:S65"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="L53:M53"/>
     <mergeCell ref="L37:M37"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I57:K57"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="A36:F36"/>

</xml_diff>

<commit_message>
nuevas pruebas ann, modificacion datetime rf
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{189458F5-4F8E-4986-BC82-CB0A689082A1}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE46D0D9-D9BA-4A13-A11D-EA4BD2D511FA}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="345" windowWidth="13500" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>0.9944</t>
+  </si>
+  <si>
+    <t>7246seg</t>
+  </si>
+  <si>
+    <t>1059seg</t>
+  </si>
+  <si>
+    <t>2383seg</t>
+  </si>
+  <si>
+    <t>0.9948</t>
   </si>
 </sst>
 </file>
@@ -450,9 +462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -490,7 +502,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -596,7 +608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -738,7 +750,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -748,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1107,12 @@
       <c r="C28">
         <v>8</v>
       </c>
+      <c r="D28">
+        <v>376312</v>
+      </c>
+      <c r="E28">
+        <v>1741</v>
+      </c>
       <c r="F28" s="2" t="s">
         <v>65</v>
       </c>
@@ -1162,6 +1180,9 @@
       <c r="M37" t="s">
         <v>40</v>
       </c>
+      <c r="N37" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D38">
@@ -1176,10 +1197,28 @@
       <c r="H38" t="s">
         <v>48</v>
       </c>
+      <c r="L38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M38" t="s">
+        <v>58</v>
+      </c>
+      <c r="N38" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>49</v>
+      </c>
+      <c r="L39" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39" t="s">
+        <v>58</v>
+      </c>
+      <c r="N39" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,6 +1442,12 @@
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
+      <c r="L68" t="s">
+        <v>73</v>
+      </c>
+      <c r="M68" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">

</xml_diff>

<commit_message>
modificaciones codigo, creacion mlp
</commit_message>
<xml_diff>
--- a/den2ne/ResultadosML.xlsx
+++ b/den2ne/ResultadosML.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/p_bartolome_edu_uah_es/Documents/Todo/TFM/den2ne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="321" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE46D0D9-D9BA-4A13-A11D-EA4BD2D511FA}"/>
+  <xr:revisionPtr revIDLastSave="423" documentId="10_ncr:40000_{839390AF-BA60-455E-96C4-180EB80D5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DD3394A-5762-4EDE-9A09-1B0BD7C28FBE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="1530" windowWidth="20265" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
   <si>
     <t>RESULTADOS PRUEBAS ML</t>
   </si>
@@ -259,13 +259,212 @@
   </si>
   <si>
     <t>0.9948</t>
+  </si>
+  <si>
+    <t>n_estimators = 25, criterion = 'entropy'</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Precisión: 0.976538 con parámetros {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}
+Tiempo ejecución grid search: 786.8710100650787
+--------------------------
+{'mean_fit_time': array([ 3.93946271,  3.92081642,  5.73457127,  5.92106366,  7.58088231,
+        7.69306335,  3.92641697,  4.26358666,  8.87294545,  9.97985806,
+        4.35881491,  4.99835033,  8.57220659,  8.45800657, 11.51267948,
+       11.10876889,  4.47397842,  4.84960222, 11.68690648, 12.37679181]), 'std_fit_time': array([0.35771976, 0.31606951, 0.19131552, 0.32361589, 0.71522803,
+       0.36175138, 0.04787848, 0.02831766, 0.69190425, 0.35206362,
+       0.51732651, 0.53883335, 1.20864354, 1.32574771, 0.89602182,
+       0.84332677, 0.11648498, 0.12411414, 0.57501269, 0.49268561]), 'mean_score_time': array([0.16318955, 0.15908413, 0.32199864, 0.33283892, 
+0.47973375,
+       0.45655594, 0.1952107 , 0.20174503, 0.59805145, 0.60064344,
+       0.24159422, 0.27124195, 0.80330291, 0.75283799, 1.34243693,
+       1.27680287, 0.34210496, 0.35037923, 1.36548772, 1.35902948]), 'std_score_time': array([0.00720741, 0.00834704, 0.00741457, 0.01600619, 0.01452746,
+       0.00791887, 0.00665817, 0.00490412, 0.01050452, 0.01013901,
+       0.01833964, 0.02775899, 0.07992402, 0.06757841, 0.05583187,
+       0.06369426, 0.0055352 , 0.00541637, 0.04559452, 0.05914715]), 'param_activation': masked_array(data=['relu', 'relu', 'relu', 'relu', 'relu', 'relu', 'relu',
+                   'relu', 'relu', 'relu', 'tanh', 'tanh', 'tanh', 'tanh',
+                   'tanh', 'tanh', 'tanh', 'tanh', 'tanh', 'tanh'],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'param_hidden_layer_sizes': masked_array(data=[(10,), (10,), (50,), (50,), (100,), (100,), (10, 10),
+                   (10, 10), (50, 50), (50, 50), (10,), (10,), (50,),
+                   (50,), (100,), (100,), (10, 10), (10, 10), (50, 50),
+                   (50, 50)],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'param_solver': masked_array(data=['sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam', 'sgd',
+                   'adam', 'sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam',
+                   'sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam'],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'params': [{'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}], 'split0_test_score': array([0.97653855, 0.97653855, 0.97653855, 0.97659551, 0.97653855,
+       0.97186231, 0.97653855, 0.97685185, 0.97653855, 0.97653855,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855]), 'split1_test_score': array([0.97653855, 0.9765515 , 0.97653855, 0.97674828, 0.97653855,
+       0.97569186, 0.97653855, 0.943489  , 0.97653855, 0.97653855,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855]), 'split2_test_score': array([0.97653855, 0.94469043, 0.97653855, 0.97471829, 0.97653855,
+       0.97599739, 0.97653855, 0.97682596, 0.97653855, 0.97652301,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855,
+       0.97653855, 0.97653855, 0.97653855, 0.97653855, 0.97653855]), 'split3_test_score': array([0.97653855, 0.93115886, 0.97653855, 0.75348517, 0.58026763,
+       0.97245526, 0.9753423 , 0.84561169, 0.97653855, 0.65112064,
+       0.97653855, 0.97653855, 0.97653855, 0.96524671, 0.97653855,
+       0.93743527, 0.97653855, 0.57985075, 0.97653855, 0.579742  ]), 'split4_test_score': array([0.97653596, 0.97634435, 0.97653596, 0.35169391, 0.97653596,
+       0.57871147, 0.97653596, 0.97666025, 0.97653596, 0.83434315,
+       0.97653596, 0.97653596, 0.97653596, 0.97653596, 0.97653596,
+       0.97539927, 0.97653596, 0.97653596, 0.97653596, 0.97653596]), 'mean_test_score': array([0.97653803, 0.96105674, 0.97653803, 0.80664823, 
+0.89728385,
+       0.89494366, 0.97629878, 0.94388775, 0.97653803, 0.88301278,
+       0.97653803, 0.97653803, 0.97653803, 0.97427966, 0.97653803,
+       0.96849004, 0.97653803, 0.89720047, 0.97653803, 0.89717872]), 'std_test_score': array([1.03571133e-06, 1.93660766e-02, 1.03571133e-06, 2.43258463e-01,
+       1.58508110e-01, 1.58124825e-01, 4.78240756e-04, 5.08014504e-02,
+       1.03571133e-06, 1.28359651e-01, 1.03571133e-06, 1.03571133e-06,
+       1.03571133e-06, 4.51647828e-03, 1.03571133e-06, 1.55336523e-02,
+       1.03571133e-06, 1.58674859e-01, 1.03571133e-06, 1.58718359e-01]), 'rank_test_score': array([ 1, 13,  1, 20, 15, 18, 10, 14,  1, 19,  1, 
+ 1,  1, 11,  1, 12,  1,
+       16,  1, 17])}
+0.976538 || 0.000001 --- {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}
+0.961057 || 0.019366 --- {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}
+0.806648 || 0.243258 --- {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'adam'}
+0.897284 || 0.158508 --- {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}
+0.894944 || 0.158125 --- {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'adam'}
+0.976299 || 0.000478 --- {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}
+0.943888 || 0.050801 --- {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}
+0.883013 || 0.128360 --- {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}
+0.974280 || 0.004516 --- {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}
+0.968490 || 0.015534 --- {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}
+0.897200 || 0.158675 --- {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}
+0.897179 || 0.158718 --- {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}</t>
+  </si>
+  <si>
+    <t>Precisión: 0.976603 con parámetros {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}
+Tiempo ejecución grid search: 14305.887028217316
+--------------------------
+{'mean_fit_time': array([ 56.48764892,  94.41483531, 142.95807862, 157.42596817,
+       169.96599994, 236.0400351 ,  53.66625361, 149.0266398 ,
+       166.01915889, 333.29285645,  43.09045324,  40.1185266 ,
+        69.71501379, 168.36691504, 131.01714177, 223.06044669,
+        48.41218557,  55.44629765, 154.76759939, 319.08375731]), 'std_fit_time': array([ 44.75224734,  29.09250309,  60.54630823,  42.01168986,
+        80.27505978,  67.86969746,  21.80713005,  20.51092235,
+       118.1826229 ,  76.4252351 ,  11.91948986,   1.0180336 ,
+         0.70861904,  38.82720646,  47.17838506,  41.62285576,
+         0.80234368,   7.45207027,  55.87735033, 117.69445236]), 'mean_score_time': array([0.14996214, 0.14232354, 0.30997   , 0.31629415, 0.46389179,
+       0.47711806, 0.19541187, 0.20527582, 0.61883922, 0.62509584,
+       0.20691886, 0.2183147 , 0.67197037, 0.70312614, 1.29879284,
+       1.26223378, 0.34619536, 0.34923344, 1.41364527, 1.39799185]), 'std_score_time': array([0.01144729, 0.00583354, 0.01887662, 0.01377622, 0.01829944,
+       0.00869271, 0.01124184, 0.00898312, 0.0242681 , 0.02584998,
+       0.00428365, 0.00605122, 0.00819424, 0.03456735, 0.05780707,
+       0.06279201, 0.00797629, 0.00779207, 0.08406714, 0.06575258]), 'param_activation': masked_array(data=['relu', 'relu', 'relu', 'relu', 'relu', 'relu', 'relu',
+                   'relu', 'relu', 'relu', 'tanh', 'tanh', 'tanh', 'tanh',
+                   'tanh', 'tanh', 'tanh', 'tanh', 'tanh', 'tanh'],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'param_hidden_layer_sizes': masked_array(data=[(10,), (10,), (50,), (50,), (100,), (100,), (10, 10),
+                   (10, 10), (50, 50), (50, 50), (10,), (10,), (50,),
+                   (50,), (100,), (100,), (10, 10), (10, 10), (50, 50),
+                   (50, 50)],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'param_solver': masked_array(data=['sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam', 'sgd',
+                   'adam', 'sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam',
+                   'sgd', 'adam', 'sgd', 'adam', 'sgd', 'adam'],
+             mask=[False, False, False, False, False, False, False, False,
+                   False, False, False, False, False, False, False, False,
+                   False, False, False, False],
+       fill_value='?',
+            dtype=object), 'params': [{'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'adam'}, {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}, 
+{'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}, {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}, {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}, {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}], 'split0_test_score': array([0.97653855, 0.97818533, 0.97672498, 0.97842872, 0.97653855,
+       0.97855819, 0.97653855, 0.97812578, 0.97653855, 0.97855301,
+       0.97653855, 0.97653855, 0.97653855, 0.97688033, 0.97653855,
+       0.97719105, 0.97653855, 0.97653855, 0.97653855, 0.97653855]), 'split1_test_score': array([0.97653855, 0.97732828, 0.97691399, 0.97880676, 0.97653855,
+       0.97853747, 0.97653855, 0.97854006, 0.9768648 , 0.97840024,
+       0.97653855, 0.97653855, 0.97653855, 0.97671462, 0.97653855,
+       0.9770098 , 0.97653855, 0.97653855, 0.97653855, 0.9771289 ]), 'split2_test_score': array([0.97653855, 0.97794194, 0.97653855, 0.97678453, 0.97679489,
+       0.97797819, 0.97653855, 0.9780714 , 0.97653855, 0.97847274,
+       0.97653855, 0.97653855, 0.97653855, 0.97703569, 0.97653855,
+       0.97690882, 0.97653855, 0.97653855, 0.97653855, 0.97796524]), 'split3_test_score': array([0.97653855, 0.57883576, 0.6962906 , 0.57853281, 0.57878397,
+       0.74065529, 0.60887656, 0.58393664, 0.97653855, 0.5786312 ,
+       0.58204646, 0.588776  , 0.97653855, 0.58329967, 0.57989218,
+       0.57913093, 0.97653855, 0.57931995, 0.58022361, 0.58799403]), 'split4_test_score': array([0.96831759, 0.83808207, 0.85028793, 0.83211119, 0.71965884,
+       0.87205081, 0.97653596, 0.56568481, 0.97653596, 0.58137066,
+       0.97653596, 0.97653596, 0.97653596, 0.97693212, 0.97653596,
+       0.97538632, 0.97653596, 0.97653596, 0.97653596, 0.58273521]), 'mean_test_score': array([0.97489436, 0.87007467, 0.89535121, 0.8689328 , 0.84566296,
+       0.90955599, 0.90300563, 0.81687174, 0.97660328, 0.81908557,
+       0.89763961, 0.89898552, 0.97653803, 0.89817249, 0.89720876,
+       0.89712538, 0.97653803, 0.89709431, 0.89727504, 0.82047239]), 'std_test_score': array([3.28838346e-03, 1.55351363e-01, 1.10924648e-01, 1.55808615e-01,
+       1.66465525e-01, 9.39525715e-02, 1.47064535e-01, 1.97726314e-01,
+       1.30762400e-04, 1.95213718e-01, 1.57796576e-01, 1.55104762e-01,
+       1.03571133e-06, 1.57436442e-01, 1.58658288e-01, 1.58998535e-01,
+       1.03571133e-06, 1.58887180e-01, 1.58525717e-01, 1.91972425e-01]), 'rank_test_score': array([ 4, 15, 14, 16, 17,  5,  6, 20,  1, 19,  9,  7,  2,  8, 11, 12,  2,
+       13, 10, 18])}
+0.974894 || 0.003288 --- {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}
+0.870075 || 0.155351 --- {'activation': 'relu', 'hidden_layer_sizes': (10,), 'solver': 'adam'}
+0.895351 || 0.110925 --- {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}
+0.868933 || 0.155809 --- {'activation': 'relu', 'hidden_layer_sizes': (50,), 'solver': 'adam'}
+0.845663 || 0.166466 --- {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}
+0.909556 || 0.093953 --- {'activation': 'relu', 'hidden_layer_sizes': (100,), 'solver': 'adam'}
+0.903006 || 0.147065 --- {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}
+0.816872 || 0.197726 --- {'activation': 'relu', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}
+0.976603 || 0.000131 --- {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}
+0.819086 || 0.195214 --- {'activation': 'relu', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}
+0.897640 || 0.157797 --- {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'sgd'}
+0.898986 || 0.155105 --- {'activation': 'tanh', 'hidden_layer_sizes': (10,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'sgd'}
+0.898172 || 0.157436 --- {'activation': 'tanh', 'hidden_layer_sizes': (50,), 'solver': 'adam'}
+0.897209 || 0.158658 --- {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'sgd'}
+0.897125 || 0.158999 --- {'activation': 'tanh', 'hidden_layer_sizes': (100,), 'solver': 'adam'}
+0.976538 || 0.000001 --- {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'sgd'}
+0.897094 || 0.158887 --- {'activation': 'tanh', 'hidden_layer_sizes': (10, 10), 'solver': 'adam'}
+0.897275 || 0.158526 --- {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'sgd'}
+0.820472 || 0.191972 --- {'activation': 'tanh', 'hidden_layer_sizes': (50, 50), 'solver': 'adam'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +508,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -361,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,6 +596,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S82"/>
+  <dimension ref="A2:AQ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7:AB71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +982,7 @@
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:43" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -785,7 +997,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -795,7 +1007,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -811,7 +1023,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -839,8 +1051,38 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AE7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="14"/>
+      <c r="AN7" s="14"/>
+      <c r="AO7" s="14"/>
+      <c r="AP7" s="14"/>
+      <c r="AQ7" s="14"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -862,8 +1104,146 @@
       <c r="H8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
+      <c r="AP9" s="14"/>
+      <c r="AQ9" s="14"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="14"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AJ10" s="14"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="14"/>
+    </row>
+    <row r="11" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="14"/>
+      <c r="AM11" s="14"/>
+      <c r="AN11" s="14"/>
+      <c r="AO11" s="14"/>
+      <c r="AP11" s="14"/>
+      <c r="AQ11" s="14"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="14"/>
+      <c r="AN12" s="14"/>
+      <c r="AO12" s="14"/>
+      <c r="AP12" s="14"/>
+      <c r="AQ12" s="14"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -878,8 +1258,34 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="14"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
+      <c r="AM13" s="14"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="14"/>
+      <c r="AP13" s="14"/>
+      <c r="AQ13" s="14"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -901,8 +1307,90 @@
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
+      <c r="AN14" s="14"/>
+      <c r="AO14" s="14"/>
+      <c r="AP14" s="14"/>
+      <c r="AQ14" s="14"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
+      <c r="AJ15" s="14"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="14"/>
+      <c r="AM15" s="14"/>
+      <c r="AN15" s="14"/>
+      <c r="AO15" s="14"/>
+      <c r="AP15" s="14"/>
+      <c r="AQ15" s="14"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
+      <c r="AJ16" s="14"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+      <c r="AP16" s="14"/>
+      <c r="AQ16" s="14"/>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -916,8 +1404,34 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14"/>
+      <c r="AH17" s="14"/>
+      <c r="AI17" s="14"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="14"/>
+      <c r="AM17" s="14"/>
+      <c r="AN17" s="14"/>
+      <c r="AO17" s="14"/>
+      <c r="AP17" s="14"/>
+      <c r="AQ17" s="14"/>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -931,8 +1445,34 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="14"/>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -954,8 +1494,34 @@
       <c r="G19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="14"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="14"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="14"/>
+      <c r="AM19" s="14"/>
+      <c r="AN19" s="14"/>
+      <c r="AO19" s="14"/>
+      <c r="AP19" s="14"/>
+      <c r="AQ19" s="14"/>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -977,8 +1543,34 @@
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+      <c r="AP20" s="14"/>
+      <c r="AQ20" s="14"/>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1000,8 +1592,62 @@
       <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AE21" s="14"/>
+      <c r="AF21" s="14"/>
+      <c r="AG21" s="14"/>
+      <c r="AH21" s="14"/>
+      <c r="AI21" s="14"/>
+      <c r="AJ21" s="14"/>
+      <c r="AK21" s="14"/>
+      <c r="AL21" s="14"/>
+      <c r="AM21" s="14"/>
+      <c r="AN21" s="14"/>
+      <c r="AO21" s="14"/>
+      <c r="AP21" s="14"/>
+      <c r="AQ21" s="14"/>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AE22" s="14"/>
+      <c r="AF22" s="14"/>
+      <c r="AG22" s="14"/>
+      <c r="AH22" s="14"/>
+      <c r="AI22" s="14"/>
+      <c r="AJ22" s="14"/>
+      <c r="AK22" s="14"/>
+      <c r="AL22" s="14"/>
+      <c r="AM22" s="14"/>
+      <c r="AN22" s="14"/>
+      <c r="AO22" s="14"/>
+      <c r="AP22" s="14"/>
+      <c r="AQ22" s="14"/>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1014,8 +1660,34 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="14"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="14"/>
+      <c r="AM23" s="14"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="14"/>
+      <c r="AP23" s="14"/>
+      <c r="AQ23" s="14"/>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -1032,8 +1704,34 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="14"/>
+      <c r="AG24" s="14"/>
+      <c r="AH24" s="14"/>
+      <c r="AI24" s="14"/>
+      <c r="AJ24" s="14"/>
+      <c r="AK24" s="14"/>
+      <c r="AL24" s="14"/>
+      <c r="AM24" s="14"/>
+      <c r="AN24" s="14"/>
+      <c r="AO24" s="14"/>
+      <c r="AP24" s="14"/>
+      <c r="AQ24" s="14"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1058,8 +1756,34 @@
       <c r="H25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="14"/>
+      <c r="AG25" s="14"/>
+      <c r="AH25" s="14"/>
+      <c r="AI25" s="14"/>
+      <c r="AJ25" s="14"/>
+      <c r="AK25" s="14"/>
+      <c r="AL25" s="14"/>
+      <c r="AM25" s="14"/>
+      <c r="AN25" s="14"/>
+      <c r="AO25" s="14"/>
+      <c r="AP25" s="14"/>
+      <c r="AQ25" s="14"/>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1081,8 +1805,34 @@
       <c r="G26" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="13"/>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14"/>
+      <c r="AG26" s="14"/>
+      <c r="AH26" s="14"/>
+      <c r="AI26" s="14"/>
+      <c r="AJ26" s="14"/>
+      <c r="AK26" s="14"/>
+      <c r="AL26" s="14"/>
+      <c r="AM26" s="14"/>
+      <c r="AN26" s="14"/>
+      <c r="AO26" s="14"/>
+      <c r="AP26" s="14"/>
+      <c r="AQ26" s="14"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -1096,8 +1846,34 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="14"/>
+      <c r="AG27" s="14"/>
+      <c r="AH27" s="14"/>
+      <c r="AI27" s="14"/>
+      <c r="AJ27" s="14"/>
+      <c r="AK27" s="14"/>
+      <c r="AL27" s="14"/>
+      <c r="AM27" s="14"/>
+      <c r="AN27" s="14"/>
+      <c r="AO27" s="14"/>
+      <c r="AP27" s="14"/>
+      <c r="AQ27" s="14"/>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1119,12 +1895,204 @@
       <c r="G28" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="13"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14"/>
+      <c r="AG28" s="14"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
+      <c r="AK28" s="14"/>
+      <c r="AL28" s="14"/>
+      <c r="AM28" s="14"/>
+      <c r="AN28" s="14"/>
+      <c r="AO28" s="14"/>
+      <c r="AP28" s="14"/>
+      <c r="AQ28" s="14"/>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="35" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13"/>
+      <c r="AE29" s="14"/>
+      <c r="AF29" s="14"/>
+      <c r="AG29" s="14"/>
+      <c r="AH29" s="14"/>
+      <c r="AI29" s="14"/>
+      <c r="AJ29" s="14"/>
+      <c r="AK29" s="14"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="14"/>
+      <c r="AN29" s="14"/>
+      <c r="AO29" s="14"/>
+      <c r="AP29" s="14"/>
+      <c r="AQ29" s="14"/>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="13"/>
+      <c r="AE30" s="14"/>
+      <c r="AF30" s="14"/>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="14"/>
+      <c r="AI30" s="14"/>
+      <c r="AJ30" s="14"/>
+      <c r="AK30" s="14"/>
+      <c r="AL30" s="14"/>
+      <c r="AM30" s="14"/>
+      <c r="AN30" s="14"/>
+      <c r="AO30" s="14"/>
+      <c r="AP30" s="14"/>
+      <c r="AQ30" s="14"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AE31" s="14"/>
+      <c r="AF31" s="14"/>
+      <c r="AG31" s="14"/>
+      <c r="AH31" s="14"/>
+      <c r="AI31" s="14"/>
+      <c r="AJ31" s="14"/>
+      <c r="AK31" s="14"/>
+      <c r="AL31" s="14"/>
+      <c r="AM31" s="14"/>
+      <c r="AN31" s="14"/>
+      <c r="AO31" s="14"/>
+      <c r="AP31" s="14"/>
+      <c r="AQ31" s="14"/>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AE32" s="14"/>
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="14"/>
+      <c r="AH32" s="14"/>
+      <c r="AI32" s="14"/>
+      <c r="AJ32" s="14"/>
+      <c r="AK32" s="14"/>
+      <c r="AL32" s="14"/>
+      <c r="AM32" s="14"/>
+      <c r="AN32" s="14"/>
+      <c r="AO32" s="14"/>
+      <c r="AP32" s="14"/>
+      <c r="AQ32" s="14"/>
+    </row>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="13"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="14"/>
+      <c r="AG33" s="14"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="14"/>
+      <c r="AJ33" s="14"/>
+      <c r="AK33" s="14"/>
+      <c r="AL33" s="14"/>
+      <c r="AM33" s="14"/>
+      <c r="AN33" s="14"/>
+      <c r="AO33" s="14"/>
+      <c r="AP33" s="14"/>
+      <c r="AQ33" s="14"/>
+    </row>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="13"/>
+      <c r="AA34" s="13"/>
+      <c r="AB34" s="13"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+      <c r="AK34" s="14"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="14"/>
+      <c r="AN34" s="14"/>
+      <c r="AO34" s="14"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="14"/>
+    </row>
+    <row r="35" spans="1:43" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>30</v>
       </c>
@@ -1133,8 +2101,34 @@
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+      <c r="W35" s="13"/>
+      <c r="X35" s="13"/>
+      <c r="Y35" s="13"/>
+      <c r="Z35" s="13"/>
+      <c r="AA35" s="13"/>
+      <c r="AB35" s="13"/>
+      <c r="AE35" s="14"/>
+      <c r="AF35" s="14"/>
+      <c r="AG35" s="14"/>
+      <c r="AH35" s="14"/>
+      <c r="AI35" s="14"/>
+      <c r="AJ35" s="14"/>
+      <c r="AK35" s="14"/>
+      <c r="AL35" s="14"/>
+      <c r="AM35" s="14"/>
+      <c r="AN35" s="14"/>
+      <c r="AO35" s="14"/>
+      <c r="AP35" s="14"/>
+      <c r="AQ35" s="14"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1160,8 +2154,34 @@
         <v>35</v>
       </c>
       <c r="M36" s="11"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="13"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="14"/>
+      <c r="AJ36" s="14"/>
+      <c r="AK36" s="14"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="14"/>
+      <c r="AN36" s="14"/>
+      <c r="AO36" s="14"/>
+      <c r="AP36" s="14"/>
+      <c r="AQ36" s="14"/>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>377071</v>
       </c>
@@ -1183,8 +2203,34 @@
       <c r="N37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="13"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+      <c r="AK37" s="14"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="14"/>
+      <c r="AN37" s="14"/>
+      <c r="AO37" s="14"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="14"/>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>377144</v>
       </c>
@@ -1206,8 +2252,34 @@
       <c r="N38" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="13"/>
+      <c r="AE38" s="14"/>
+      <c r="AF38" s="14"/>
+      <c r="AG38" s="14"/>
+      <c r="AH38" s="14"/>
+      <c r="AI38" s="14"/>
+      <c r="AJ38" s="14"/>
+      <c r="AK38" s="14"/>
+      <c r="AL38" s="14"/>
+      <c r="AM38" s="14"/>
+      <c r="AN38" s="14"/>
+      <c r="AO38" s="14"/>
+      <c r="AP38" s="14"/>
+      <c r="AQ38" s="14"/>
+    </row>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>49</v>
       </c>
@@ -1220,14 +2292,66 @@
       <c r="N39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="13"/>
+      <c r="AA39" s="13"/>
+      <c r="AB39" s="13"/>
+      <c r="AE39" s="14"/>
+      <c r="AF39" s="14"/>
+      <c r="AG39" s="14"/>
+      <c r="AH39" s="14"/>
+      <c r="AI39" s="14"/>
+      <c r="AJ39" s="14"/>
+      <c r="AK39" s="14"/>
+      <c r="AL39" s="14"/>
+      <c r="AM39" s="14"/>
+      <c r="AN39" s="14"/>
+      <c r="AO39" s="14"/>
+      <c r="AP39" s="14"/>
+      <c r="AQ39" s="14"/>
+    </row>
+    <row r="40" spans="1:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>53</v>
       </c>
       <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="13"/>
+      <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="13"/>
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="13"/>
+      <c r="AE40" s="14"/>
+      <c r="AF40" s="14"/>
+      <c r="AG40" s="14"/>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="14"/>
+      <c r="AJ40" s="14"/>
+      <c r="AK40" s="14"/>
+      <c r="AL40" s="14"/>
+      <c r="AM40" s="14"/>
+      <c r="AN40" s="14"/>
+      <c r="AO40" s="14"/>
+      <c r="AP40" s="14"/>
+      <c r="AQ40" s="14"/>
+    </row>
+    <row r="41" spans="1:43" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="H41" t="s">
         <v>54</v>
@@ -1237,8 +2361,118 @@
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="13"/>
+      <c r="AB41" s="13"/>
+      <c r="AE41" s="14"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14"/>
+      <c r="AH41" s="14"/>
+      <c r="AI41" s="14"/>
+      <c r="AJ41" s="14"/>
+      <c r="AK41" s="14"/>
+      <c r="AL41" s="14"/>
+      <c r="AM41" s="14"/>
+      <c r="AN41" s="14"/>
+      <c r="AO41" s="14"/>
+      <c r="AP41" s="14"/>
+      <c r="AQ41" s="14"/>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AE42" s="14"/>
+      <c r="AF42" s="14"/>
+      <c r="AG42" s="14"/>
+      <c r="AH42" s="14"/>
+      <c r="AI42" s="14"/>
+      <c r="AJ42" s="14"/>
+      <c r="AK42" s="14"/>
+      <c r="AL42" s="14"/>
+      <c r="AM42" s="14"/>
+      <c r="AN42" s="14"/>
+      <c r="AO42" s="14"/>
+      <c r="AP42" s="14"/>
+      <c r="AQ42" s="14"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="14"/>
+      <c r="AJ43" s="14"/>
+      <c r="AK43" s="14"/>
+      <c r="AL43" s="14"/>
+      <c r="AM43" s="14"/>
+      <c r="AN43" s="14"/>
+      <c r="AO43" s="14"/>
+      <c r="AP43" s="14"/>
+      <c r="AQ43" s="14"/>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+      <c r="W44" s="13"/>
+      <c r="X44" s="13"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="13"/>
+      <c r="AE44" s="14"/>
+      <c r="AF44" s="14"/>
+      <c r="AG44" s="14"/>
+      <c r="AH44" s="14"/>
+      <c r="AI44" s="14"/>
+      <c r="AJ44" s="14"/>
+      <c r="AK44" s="14"/>
+      <c r="AL44" s="14"/>
+      <c r="AM44" s="14"/>
+      <c r="AN44" s="14"/>
+      <c r="AO44" s="14"/>
+      <c r="AP44" s="14"/>
+      <c r="AQ44" s="14"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -1258,10 +2492,426 @@
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-    </row>
-    <row r="56" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="14"/>
+      <c r="AI45" s="14"/>
+      <c r="AJ45" s="14"/>
+      <c r="AK45" s="14"/>
+      <c r="AL45" s="14"/>
+      <c r="AM45" s="14"/>
+      <c r="AN45" s="14"/>
+      <c r="AO45" s="14"/>
+      <c r="AP45" s="14"/>
+      <c r="AQ45" s="14"/>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="13"/>
+      <c r="X46" s="13"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AE46" s="14"/>
+      <c r="AF46" s="14"/>
+      <c r="AG46" s="14"/>
+      <c r="AH46" s="14"/>
+      <c r="AI46" s="14"/>
+      <c r="AJ46" s="14"/>
+      <c r="AK46" s="14"/>
+      <c r="AL46" s="14"/>
+      <c r="AM46" s="14"/>
+      <c r="AN46" s="14"/>
+      <c r="AO46" s="14"/>
+      <c r="AP46" s="14"/>
+      <c r="AQ46" s="14"/>
+    </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AE47" s="14"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="14"/>
+      <c r="AH47" s="14"/>
+      <c r="AI47" s="14"/>
+      <c r="AJ47" s="14"/>
+      <c r="AK47" s="14"/>
+      <c r="AL47" s="14"/>
+      <c r="AM47" s="14"/>
+      <c r="AN47" s="14"/>
+      <c r="AO47" s="14"/>
+      <c r="AP47" s="14"/>
+      <c r="AQ47" s="14"/>
+    </row>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
+      <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AE48" s="14"/>
+      <c r="AF48" s="14"/>
+      <c r="AG48" s="14"/>
+      <c r="AH48" s="14"/>
+      <c r="AI48" s="14"/>
+      <c r="AJ48" s="14"/>
+      <c r="AK48" s="14"/>
+      <c r="AL48" s="14"/>
+      <c r="AM48" s="14"/>
+      <c r="AN48" s="14"/>
+      <c r="AO48" s="14"/>
+      <c r="AP48" s="14"/>
+      <c r="AQ48" s="14"/>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AE49" s="14"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
+      <c r="AH49" s="14"/>
+      <c r="AI49" s="14"/>
+      <c r="AJ49" s="14"/>
+      <c r="AK49" s="14"/>
+      <c r="AL49" s="14"/>
+      <c r="AM49" s="14"/>
+      <c r="AN49" s="14"/>
+      <c r="AO49" s="14"/>
+      <c r="AP49" s="14"/>
+      <c r="AQ49" s="14"/>
+    </row>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+      <c r="W50" s="13"/>
+      <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AE50" s="14"/>
+      <c r="AF50" s="14"/>
+      <c r="AG50" s="14"/>
+      <c r="AH50" s="14"/>
+      <c r="AI50" s="14"/>
+      <c r="AJ50" s="14"/>
+      <c r="AK50" s="14"/>
+      <c r="AL50" s="14"/>
+      <c r="AM50" s="14"/>
+      <c r="AN50" s="14"/>
+      <c r="AO50" s="14"/>
+      <c r="AP50" s="14"/>
+      <c r="AQ50" s="14"/>
+    </row>
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="13"/>
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="13"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="14"/>
+      <c r="AI51" s="14"/>
+      <c r="AJ51" s="14"/>
+      <c r="AK51" s="14"/>
+      <c r="AL51" s="14"/>
+      <c r="AM51" s="14"/>
+      <c r="AN51" s="14"/>
+      <c r="AO51" s="14"/>
+      <c r="AP51" s="14"/>
+      <c r="AQ51" s="14"/>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="13"/>
+      <c r="W52" s="13"/>
+      <c r="X52" s="13"/>
+      <c r="Y52" s="13"/>
+      <c r="Z52" s="13"/>
+      <c r="AA52" s="13"/>
+      <c r="AB52" s="13"/>
+      <c r="AE52" s="14"/>
+      <c r="AF52" s="14"/>
+      <c r="AG52" s="14"/>
+      <c r="AH52" s="14"/>
+      <c r="AI52" s="14"/>
+      <c r="AJ52" s="14"/>
+      <c r="AK52" s="14"/>
+      <c r="AL52" s="14"/>
+      <c r="AM52" s="14"/>
+      <c r="AN52" s="14"/>
+      <c r="AO52" s="14"/>
+      <c r="AP52" s="14"/>
+      <c r="AQ52" s="14"/>
+    </row>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="13"/>
+      <c r="W53" s="13"/>
+      <c r="X53" s="13"/>
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="13"/>
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13"/>
+      <c r="AE53" s="14"/>
+      <c r="AF53" s="14"/>
+      <c r="AG53" s="14"/>
+      <c r="AH53" s="14"/>
+      <c r="AI53" s="14"/>
+      <c r="AJ53" s="14"/>
+      <c r="AK53" s="14"/>
+      <c r="AL53" s="14"/>
+      <c r="AM53" s="14"/>
+      <c r="AN53" s="14"/>
+      <c r="AO53" s="14"/>
+      <c r="AP53" s="14"/>
+      <c r="AQ53" s="14"/>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="13"/>
+      <c r="U54" s="13"/>
+      <c r="V54" s="13"/>
+      <c r="W54" s="13"/>
+      <c r="X54" s="13"/>
+      <c r="Y54" s="13"/>
+      <c r="Z54" s="13"/>
+      <c r="AA54" s="13"/>
+      <c r="AB54" s="13"/>
+      <c r="AE54" s="14"/>
+      <c r="AF54" s="14"/>
+      <c r="AG54" s="14"/>
+      <c r="AH54" s="14"/>
+      <c r="AI54" s="14"/>
+      <c r="AJ54" s="14"/>
+      <c r="AK54" s="14"/>
+      <c r="AL54" s="14"/>
+      <c r="AM54" s="14"/>
+      <c r="AN54" s="14"/>
+      <c r="AO54" s="14"/>
+      <c r="AP54" s="14"/>
+      <c r="AQ54" s="14"/>
+    </row>
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
+      <c r="X55" s="13"/>
+      <c r="Y55" s="13"/>
+      <c r="Z55" s="13"/>
+      <c r="AA55" s="13"/>
+      <c r="AB55" s="13"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="14"/>
+      <c r="AI55" s="14"/>
+      <c r="AJ55" s="14"/>
+      <c r="AK55" s="14"/>
+      <c r="AL55" s="14"/>
+      <c r="AM55" s="14"/>
+      <c r="AN55" s="14"/>
+      <c r="AO55" s="14"/>
+      <c r="AP55" s="14"/>
+      <c r="AQ55" s="14"/>
+    </row>
+    <row r="56" spans="1:43" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="13"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="13"/>
+      <c r="W56" s="13"/>
+      <c r="X56" s="13"/>
+      <c r="Y56" s="13"/>
+      <c r="Z56" s="13"/>
+      <c r="AA56" s="13"/>
+      <c r="AB56" s="13"/>
+      <c r="AE56" s="14"/>
+      <c r="AF56" s="14"/>
+      <c r="AG56" s="14"/>
+      <c r="AH56" s="14"/>
+      <c r="AI56" s="14"/>
+      <c r="AJ56" s="14"/>
+      <c r="AK56" s="14"/>
+      <c r="AL56" s="14"/>
+      <c r="AM56" s="14"/>
+      <c r="AN56" s="14"/>
+      <c r="AO56" s="14"/>
+      <c r="AP56" s="14"/>
+      <c r="AQ56" s="14"/>
+    </row>
+    <row r="57" spans="1:43" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="13"/>
+      <c r="W57" s="13"/>
+      <c r="X57" s="13"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="13"/>
+      <c r="AA57" s="13"/>
+      <c r="AB57" s="13"/>
+      <c r="AE57" s="14"/>
+      <c r="AF57" s="14"/>
+      <c r="AG57" s="14"/>
+      <c r="AH57" s="14"/>
+      <c r="AI57" s="14"/>
+      <c r="AJ57" s="14"/>
+      <c r="AK57" s="14"/>
+      <c r="AL57" s="14"/>
+      <c r="AM57" s="14"/>
+      <c r="AN57" s="14"/>
+      <c r="AO57" s="14"/>
+      <c r="AP57" s="14"/>
+      <c r="AQ57" s="14"/>
+    </row>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="13"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="13"/>
+      <c r="W58" s="13"/>
+      <c r="X58" s="13"/>
+      <c r="Y58" s="13"/>
+      <c r="Z58" s="13"/>
+      <c r="AA58" s="13"/>
+      <c r="AB58" s="13"/>
+      <c r="AE58" s="14"/>
+      <c r="AF58" s="14"/>
+      <c r="AG58" s="14"/>
+      <c r="AH58" s="14"/>
+      <c r="AI58" s="14"/>
+      <c r="AJ58" s="14"/>
+      <c r="AK58" s="14"/>
+      <c r="AL58" s="14"/>
+      <c r="AM58" s="14"/>
+      <c r="AN58" s="14"/>
+      <c r="AO58" s="14"/>
+      <c r="AP58" s="14"/>
+      <c r="AQ58" s="14"/>
+    </row>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="13"/>
+      <c r="U59" s="13"/>
+      <c r="V59" s="13"/>
+      <c r="W59" s="13"/>
+      <c r="X59" s="13"/>
+      <c r="Y59" s="13"/>
+      <c r="Z59" s="13"/>
+      <c r="AA59" s="13"/>
+      <c r="AB59" s="13"/>
+      <c r="AE59" s="14"/>
+      <c r="AF59" s="14"/>
+      <c r="AG59" s="14"/>
+      <c r="AH59" s="14"/>
+      <c r="AI59" s="14"/>
+      <c r="AJ59" s="14"/>
+      <c r="AK59" s="14"/>
+      <c r="AL59" s="14"/>
+      <c r="AM59" s="14"/>
+      <c r="AN59" s="14"/>
+      <c r="AO59" s="14"/>
+      <c r="AP59" s="14"/>
+      <c r="AQ59" s="14"/>
+    </row>
+    <row r="60" spans="1:43" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>33</v>
       </c>
@@ -1270,8 +2920,34 @@
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="13"/>
+      <c r="U60" s="13"/>
+      <c r="V60" s="13"/>
+      <c r="W60" s="13"/>
+      <c r="X60" s="13"/>
+      <c r="Y60" s="13"/>
+      <c r="Z60" s="13"/>
+      <c r="AA60" s="13"/>
+      <c r="AB60" s="13"/>
+      <c r="AE60" s="14"/>
+      <c r="AF60" s="14"/>
+      <c r="AG60" s="14"/>
+      <c r="AH60" s="14"/>
+      <c r="AI60" s="14"/>
+      <c r="AJ60" s="14"/>
+      <c r="AK60" s="14"/>
+      <c r="AL60" s="14"/>
+      <c r="AM60" s="14"/>
+      <c r="AN60" s="14"/>
+      <c r="AO60" s="14"/>
+      <c r="AP60" s="14"/>
+      <c r="AQ60" s="14"/>
+    </row>
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>42</v>
       </c>
@@ -1286,8 +2962,34 @@
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="13"/>
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
+      <c r="W61" s="13"/>
+      <c r="X61" s="13"/>
+      <c r="Y61" s="13"/>
+      <c r="Z61" s="13"/>
+      <c r="AA61" s="13"/>
+      <c r="AB61" s="13"/>
+      <c r="AE61" s="14"/>
+      <c r="AF61" s="14"/>
+      <c r="AG61" s="14"/>
+      <c r="AH61" s="14"/>
+      <c r="AI61" s="14"/>
+      <c r="AJ61" s="14"/>
+      <c r="AK61" s="14"/>
+      <c r="AL61" s="14"/>
+      <c r="AM61" s="14"/>
+      <c r="AN61" s="14"/>
+      <c r="AO61" s="14"/>
+      <c r="AP61" s="14"/>
+      <c r="AQ61" s="14"/>
+    </row>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1313,8 +3015,34 @@
         <v>35</v>
       </c>
       <c r="M62" s="11"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="13"/>
+      <c r="U62" s="13"/>
+      <c r="V62" s="13"/>
+      <c r="W62" s="13"/>
+      <c r="X62" s="13"/>
+      <c r="Y62" s="13"/>
+      <c r="Z62" s="13"/>
+      <c r="AA62" s="13"/>
+      <c r="AB62" s="13"/>
+      <c r="AE62" s="14"/>
+      <c r="AF62" s="14"/>
+      <c r="AG62" s="14"/>
+      <c r="AH62" s="14"/>
+      <c r="AI62" s="14"/>
+      <c r="AJ62" s="14"/>
+      <c r="AK62" s="14"/>
+      <c r="AL62" s="14"/>
+      <c r="AM62" s="14"/>
+      <c r="AN62" s="14"/>
+      <c r="AO62" s="14"/>
+      <c r="AP62" s="14"/>
+      <c r="AQ62" s="14"/>
+    </row>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D63">
         <v>376752</v>
       </c>
@@ -1333,8 +3061,34 @@
       <c r="M63" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="13"/>
+      <c r="U63" s="13"/>
+      <c r="V63" s="13"/>
+      <c r="W63" s="13"/>
+      <c r="X63" s="13"/>
+      <c r="Y63" s="13"/>
+      <c r="Z63" s="13"/>
+      <c r="AA63" s="13"/>
+      <c r="AB63" s="13"/>
+      <c r="AE63" s="14"/>
+      <c r="AF63" s="14"/>
+      <c r="AG63" s="14"/>
+      <c r="AH63" s="14"/>
+      <c r="AI63" s="14"/>
+      <c r="AJ63" s="14"/>
+      <c r="AK63" s="14"/>
+      <c r="AL63" s="14"/>
+      <c r="AM63" s="14"/>
+      <c r="AN63" s="14"/>
+      <c r="AO63" s="14"/>
+      <c r="AP63" s="14"/>
+      <c r="AQ63" s="14"/>
+    </row>
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D64">
         <v>376593</v>
       </c>
@@ -1353,8 +3107,34 @@
       <c r="M64" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="13"/>
+      <c r="U64" s="13"/>
+      <c r="V64" s="13"/>
+      <c r="W64" s="13"/>
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13"/>
+      <c r="Z64" s="13"/>
+      <c r="AA64" s="13"/>
+      <c r="AB64" s="13"/>
+      <c r="AE64" s="14"/>
+      <c r="AF64" s="14"/>
+      <c r="AG64" s="14"/>
+      <c r="AH64" s="14"/>
+      <c r="AI64" s="14"/>
+      <c r="AJ64" s="14"/>
+      <c r="AK64" s="14"/>
+      <c r="AL64" s="14"/>
+      <c r="AM64" s="14"/>
+      <c r="AN64" s="14"/>
+      <c r="AO64" s="14"/>
+      <c r="AP64" s="14"/>
+      <c r="AQ64" s="14"/>
+    </row>
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>376965</v>
       </c>
@@ -1373,8 +3153,34 @@
       <c r="M65" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="13"/>
+      <c r="W65" s="13"/>
+      <c r="X65" s="13"/>
+      <c r="Y65" s="13"/>
+      <c r="Z65" s="13"/>
+      <c r="AA65" s="13"/>
+      <c r="AB65" s="13"/>
+      <c r="AE65" s="14"/>
+      <c r="AF65" s="14"/>
+      <c r="AG65" s="14"/>
+      <c r="AH65" s="14"/>
+      <c r="AI65" s="14"/>
+      <c r="AJ65" s="14"/>
+      <c r="AK65" s="14"/>
+      <c r="AL65" s="14"/>
+      <c r="AM65" s="14"/>
+      <c r="AN65" s="14"/>
+      <c r="AO65" s="14"/>
+      <c r="AP65" s="14"/>
+      <c r="AQ65" s="14"/>
+    </row>
+    <row r="66" spans="1:43" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>376555</v>
       </c>
@@ -1398,8 +3204,34 @@
       <c r="M66" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13"/>
+      <c r="U66" s="13"/>
+      <c r="V66" s="13"/>
+      <c r="W66" s="13"/>
+      <c r="X66" s="13"/>
+      <c r="Y66" s="13"/>
+      <c r="Z66" s="13"/>
+      <c r="AA66" s="13"/>
+      <c r="AB66" s="13"/>
+      <c r="AE66" s="14"/>
+      <c r="AF66" s="14"/>
+      <c r="AG66" s="14"/>
+      <c r="AH66" s="14"/>
+      <c r="AI66" s="14"/>
+      <c r="AJ66" s="14"/>
+      <c r="AK66" s="14"/>
+      <c r="AL66" s="14"/>
+      <c r="AM66" s="14"/>
+      <c r="AN66" s="14"/>
+      <c r="AO66" s="14"/>
+      <c r="AP66" s="14"/>
+      <c r="AQ66" s="14"/>
+    </row>
+    <row r="67" spans="1:43" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>374986</v>
       </c>
@@ -1423,8 +3255,34 @@
       <c r="M67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="13"/>
+      <c r="U67" s="13"/>
+      <c r="V67" s="13"/>
+      <c r="W67" s="13"/>
+      <c r="X67" s="13"/>
+      <c r="Y67" s="13"/>
+      <c r="Z67" s="13"/>
+      <c r="AA67" s="13"/>
+      <c r="AB67" s="13"/>
+      <c r="AE67" s="14"/>
+      <c r="AF67" s="14"/>
+      <c r="AG67" s="14"/>
+      <c r="AH67" s="14"/>
+      <c r="AI67" s="14"/>
+      <c r="AJ67" s="14"/>
+      <c r="AK67" s="14"/>
+      <c r="AL67" s="14"/>
+      <c r="AM67" s="14"/>
+      <c r="AN67" s="14"/>
+      <c r="AO67" s="14"/>
+      <c r="AP67" s="14"/>
+      <c r="AQ67" s="14"/>
+    </row>
+    <row r="68" spans="1:43" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D68">
         <v>376718</v>
       </c>
@@ -1448,8 +3306,118 @@
       <c r="M68" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="13"/>
+      <c r="U68" s="13"/>
+      <c r="V68" s="13"/>
+      <c r="W68" s="13"/>
+      <c r="X68" s="13"/>
+      <c r="Y68" s="13"/>
+      <c r="Z68" s="13"/>
+      <c r="AA68" s="13"/>
+      <c r="AB68" s="13"/>
+      <c r="AE68" s="14"/>
+      <c r="AF68" s="14"/>
+      <c r="AG68" s="14"/>
+      <c r="AH68" s="14"/>
+      <c r="AI68" s="14"/>
+      <c r="AJ68" s="14"/>
+      <c r="AK68" s="14"/>
+      <c r="AL68" s="14"/>
+      <c r="AM68" s="14"/>
+      <c r="AN68" s="14"/>
+      <c r="AO68" s="14"/>
+      <c r="AP68" s="14"/>
+      <c r="AQ68" s="14"/>
+    </row>
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="13"/>
+      <c r="U69" s="13"/>
+      <c r="V69" s="13"/>
+      <c r="W69" s="13"/>
+      <c r="X69" s="13"/>
+      <c r="Y69" s="13"/>
+      <c r="Z69" s="13"/>
+      <c r="AA69" s="13"/>
+      <c r="AB69" s="13"/>
+      <c r="AE69" s="14"/>
+      <c r="AF69" s="14"/>
+      <c r="AG69" s="14"/>
+      <c r="AH69" s="14"/>
+      <c r="AI69" s="14"/>
+      <c r="AJ69" s="14"/>
+      <c r="AK69" s="14"/>
+      <c r="AL69" s="14"/>
+      <c r="AM69" s="14"/>
+      <c r="AN69" s="14"/>
+      <c r="AO69" s="14"/>
+      <c r="AP69" s="14"/>
+      <c r="AQ69" s="14"/>
+    </row>
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="13"/>
+      <c r="U70" s="13"/>
+      <c r="V70" s="13"/>
+      <c r="W70" s="13"/>
+      <c r="X70" s="13"/>
+      <c r="Y70" s="13"/>
+      <c r="Z70" s="13"/>
+      <c r="AA70" s="13"/>
+      <c r="AB70" s="13"/>
+      <c r="AE70" s="14"/>
+      <c r="AF70" s="14"/>
+      <c r="AG70" s="14"/>
+      <c r="AH70" s="14"/>
+      <c r="AI70" s="14"/>
+      <c r="AJ70" s="14"/>
+      <c r="AK70" s="14"/>
+      <c r="AL70" s="14"/>
+      <c r="AM70" s="14"/>
+      <c r="AN70" s="14"/>
+      <c r="AO70" s="14"/>
+      <c r="AP70" s="14"/>
+      <c r="AQ70" s="14"/>
+    </row>
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+      <c r="U71" s="13"/>
+      <c r="V71" s="13"/>
+      <c r="W71" s="13"/>
+      <c r="X71" s="13"/>
+      <c r="Y71" s="13"/>
+      <c r="Z71" s="13"/>
+      <c r="AA71" s="13"/>
+      <c r="AB71" s="13"/>
+      <c r="AE71" s="14"/>
+      <c r="AF71" s="14"/>
+      <c r="AG71" s="14"/>
+      <c r="AH71" s="14"/>
+      <c r="AI71" s="14"/>
+      <c r="AJ71" s="14"/>
+      <c r="AK71" s="14"/>
+      <c r="AL71" s="14"/>
+      <c r="AM71" s="14"/>
+      <c r="AN71" s="14"/>
+      <c r="AO71" s="14"/>
+      <c r="AP71" s="14"/>
+      <c r="AQ71" s="14"/>
+    </row>
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>46</v>
       </c>
@@ -1473,7 +3441,7 @@
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>44</v>
       </c>
@@ -1484,7 +3452,7 @@
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>45</v>
       </c>
@@ -1500,15 +3468,100 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L82" s="4"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>79</v>
+      </c>
+      <c r="I85" t="s">
+        <v>80</v>
+      </c>
+      <c r="J85" t="s">
+        <v>81</v>
+      </c>
+      <c r="K85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <v>376684</v>
+      </c>
+      <c r="I86">
+        <v>460</v>
+      </c>
+      <c r="J86">
+        <v>7015</v>
+      </c>
+      <c r="K86">
+        <v>2049</v>
+      </c>
+      <c r="M86" t="s">
+        <v>75</v>
+      </c>
+      <c r="N86">
+        <f>(K86+H86)/(H86+I86+J86+K86)</f>
+        <v>0.98064514458530117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M87" t="s">
+        <v>76</v>
+      </c>
+      <c r="N87">
+        <f>K86/(K86+I86)</f>
+        <v>0.8166600239139099</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M88" t="s">
+        <v>77</v>
+      </c>
+      <c r="N88">
+        <f>K86/(K86+J86)</f>
+        <v>0.22605913503971756</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M89" t="s">
+        <v>78</v>
+      </c>
+      <c r="N89">
+        <f>2*N87*N88/(N87+N88)</f>
+        <v>0.35410006048561304</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K94" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="AE7:AQ71"/>
+    <mergeCell ref="P7:AB71"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="A35:F35"/>

</xml_diff>